<commit_message>
customer sms after payment confirmation
</commit_message>
<xml_diff>
--- a/Data Files/File Upload Center/File Upload Center.xlsx
+++ b/Data Files/File Upload Center/File Upload Center.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dennis.gituto\git\MKOPA_Regression_Test_Channel\Data Files\File Upload Center\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal.Kipkemoi\git\MKOPA_Regression_Test_Channel\Data Files\File Upload Center\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>filePath</t>
   </si>
   <si>
-    <t>C:\Users\dennis.gituto\git\MKOPA_Regression_Test_Channel\FilesToUpload\Mpesalatest File.csv</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -41,13 +38,16 @@
     <t>Perfect and Precise</t>
   </si>
   <si>
-    <t>polr32</t>
+    <t>C:\Users\Pascal.Kipkemoi\git\MKOPA_Regression_Test_Channel\FilesToUpload\Mpesalatest File.csv</t>
+  </si>
+  <si>
+    <t>polr780</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,36 +358,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88" customWidth="1"/>
-    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="2" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Credit purchase payment upload
</commit_message>
<xml_diff>
--- a/Data Files/File Upload Center/File Upload Center.xlsx
+++ b/Data Files/File Upload Center/File Upload Center.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dennis.gituto\git\MKOPA_Regression_Test_Channel\Data Files\File Upload Center\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stellah.ireri\git\MKOPA_Regression_Test_Channel\Data Files\File Upload Center\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7632"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>filePath</t>
   </si>
   <si>
-    <t>C:\Users\dennis.gituto\git\MKOPA_Regression_Test_Channel\FilesToUpload\Mpesalatest File.csv</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -42,6 +39,9 @@
   </si>
   <si>
     <t>polr32</t>
+  </si>
+  <si>
+    <t>C:\Users\stellah.ireri\git\MKOPA_Regression_Test_Channel\FilesToUpload\Mpesalatest File.csv</t>
   </si>
 </sst>
 </file>
@@ -362,35 +362,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88" customWidth="1"/>
-    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="2" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>